<commit_message>
Resolve wait in test scripts
</commit_message>
<xml_diff>
--- a/TestScripts/SystemPages/SystemPages.xlsx
+++ b/TestScripts/SystemPages/SystemPages.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ActiTest\selenium_project\TestScripts\SystemPages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{649E71A2-7735-49A6-9C5B-E39370BC6395}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC59196E-A206-47CA-9C09-49720E0633D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>TESTCASEID</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>customer_$R</t>
+  </si>
+  <si>
+    <t>TC8</t>
+  </si>
+  <si>
+    <t>TC9</t>
   </si>
 </sst>
 </file>
@@ -487,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,13 +541,10 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -549,81 +552,95 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
         <v>24</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added testcase for logout
</commit_message>
<xml_diff>
--- a/TestScripts/SystemPages/SystemPages.xlsx
+++ b/TestScripts/SystemPages/SystemPages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ActiTest\selenium_project\TestScripts\SystemPages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC59196E-A206-47CA-9C09-49720E0633D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A10B7B-1685-4C14-872A-3386ED238989}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>TESTCASEID</t>
   </si>
@@ -118,6 +118,21 @@
   </si>
   <si>
     <t>TC9</t>
+  </si>
+  <si>
+    <t>TC10</t>
+  </si>
+  <si>
+    <t>Click on Logout</t>
+  </si>
+  <si>
+    <t>xpath~//*[@id="logoutLink"]</t>
+  </si>
+  <si>
+    <t>TC11</t>
+  </si>
+  <si>
+    <t>TC12</t>
   </si>
 </sst>
 </file>
@@ -493,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,6 +659,42 @@
         <v>25</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>